<commit_message>
add: input column converters
</commit_message>
<xml_diff>
--- a/input/emails2query_template.xlsx
+++ b/input/emails2query_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antoniosanmateuserralta/dev/JOOR/emails2query/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD47DD5-32E7-2D4A-A802-05B5410430FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD101B9E-8F44-D74F-8551-9C243ABF451C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17460" yWindow="4880" windowWidth="16080" windowHeight="20180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,60 +31,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>retailer_id</t>
   </si>
   <si>
     <t>additional_emails</t>
-  </si>
-  <si>
-    <t>techeberrymonge@galerieslafayette.com, ccornet@galerieslafayette.com</t>
-  </si>
-  <si>
-    <t>audrey@influenceu.com</t>
-  </si>
-  <si>
-    <t>Robert@xhibition.co</t>
-  </si>
-  <si>
-    <t>Tommy@shoptrafficla.com, davina@shoptrafficla.com</t>
-  </si>
-  <si>
-    <t>dom@somewhereofficial.com</t>
-  </si>
-  <si>
-    <t>parishandsome@gmail.com</t>
-  </si>
-  <si>
-    <t>Mkartal@printemps.com, atistounet@printemps.fr, mlataste@printemps.fr</t>
-  </si>
-  <si>
-    <t>prune@serie-noire.fr</t>
-  </si>
-  <si>
-    <t>charlotte@joggingjogging.com</t>
-  </si>
-  <si>
-    <t>achats@archive1820.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jgrodenic@lebonmarche.fr, icarrazza@lebonmarche.fr, </t>
-  </si>
-  <si>
-    <t>manshop@lespionne.com, office@lespionne.com</t>
-  </si>
-  <si>
-    <t>l.coulier@lvmh.fr</t>
-  </si>
-  <si>
-    <t>contact@capsulebyeso.com</t>
-  </si>
-  <si>
-    <t>alafarge@the-broken-arm.com</t>
-  </si>
-  <si>
-    <t>office@unitedlegend.com</t>
   </si>
   <si>
     <t>additional_buyers</t>
@@ -606,7 +558,7 @@
   <dimension ref="A1:C466"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A2" sqref="A2:XFD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -620,139 +572,56 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>404064</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>2</v>
-      </c>
+      <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>630781</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>3</v>
-      </c>
+      <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>216028</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>4</v>
-      </c>
+      <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>5268</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>481981</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>6</v>
-      </c>
+      <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>131591</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>7</v>
-      </c>
+      <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>4068</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>4464</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>591842</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>10</v>
-      </c>
+      <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>133889</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="C11" s="5"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>2887</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>2939</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>206679</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>726130</v>
-      </c>
-      <c r="C15" t="s">
-        <v>15</v>
-      </c>
+      <c r="C14" s="5"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>91510</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>100165</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>17</v>
-      </c>
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C17" s="5"/>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" s="3"/>
@@ -1585,23 +1454,6 @@
       <formula>AND(LEN($C17)&gt;0)*(ISBLANK($O17))</formula>
     </cfRule>
   </conditionalFormatting>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="techeberrymonge@galerieslafayette.com" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="C5" r:id="rId4" display="Tommy@shoptrafficla.com" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="C6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="C7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="C8" r:id="rId7" display="Mkartal@printemps.com" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="C9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="C10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="C11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="C12" r:id="rId11" display="jgrodenic@lebonmarche.fr" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="C13" r:id="rId12" display="manshop@lespionne.com" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="C14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="C16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="C17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>